<commit_message>
tutorial model in process
</commit_message>
<xml_diff>
--- a/tutorial/CovidContagion/data/input/simulator_scenarios.xlsx
+++ b/tutorial/CovidContagion/data/input/simulator_scenarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/ABM4ALL/Melodie/tutorial/VirusContagion/data/excel_source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/ABM4ALL/Melodie/tutorial/CovidContagion/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B0E866-00EB-5C46-8942-1B85C4D3152E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07DF48A-464F-CD4F-8115-7EEA2642CC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -43,7 +43,19 @@
     <t>initial_infected_percentage</t>
   </si>
   <si>
-    <t>infection_probability</t>
+    <t>period_hours</t>
+  </si>
+  <si>
+    <t>young_percentage</t>
+  </si>
+  <si>
+    <t>infection_prob</t>
+  </si>
+  <si>
+    <t>reinfection_prob</t>
+  </si>
+  <si>
+    <t>vaccinated_infection_prob</t>
   </si>
 </sst>
 </file>
@@ -363,22 +375,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="334" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="23.5" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10" customWidth="1"/>
+    <col min="8" max="9" width="23.5" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,22 +404,34 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -415,19 +442,31 @@
         <v>100</v>
       </c>
       <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
         <v>1000</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
       </c>
       <c r="F2">
         <v>100</v>
       </c>
-      <c r="G2" s="1">
-        <v>0.1</v>
+      <c r="G2">
+        <v>100</v>
       </c>
       <c r="H2" s="1">
         <v>0.1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K2">
+        <v>1E-3</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tutorial: covid example network setup in process
</commit_message>
<xml_diff>
--- a/tutorial/CovidContagion/data/input/simulator_scenarios.xlsx
+++ b/tutorial/CovidContagion/data/input/simulator_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/ABM4ALL/Melodie/tutorial/CovidContagion/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07DF48A-464F-CD4F-8115-7EEA2642CC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F72E9B3-9762-A14F-BF98-95BF03D62CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -56,6 +56,33 @@
   </si>
   <si>
     <t>vaccinated_infection_prob</t>
+  </si>
+  <si>
+    <t>vaccination_trust_percentage</t>
+  </si>
+  <si>
+    <t>vaccination_ad_percentage</t>
+  </si>
+  <si>
+    <t>vaccination_ad_success_prob</t>
+  </si>
+  <si>
+    <t>vaccination_action_prob</t>
+  </si>
+  <si>
+    <t>network_param_k</t>
+  </si>
+  <si>
+    <t>network_param_p</t>
+  </si>
+  <si>
+    <t>network_param_threshold</t>
+  </si>
+  <si>
+    <t>network_type</t>
+  </si>
+  <si>
+    <t>network_param_m</t>
   </si>
 </sst>
 </file>
@@ -375,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="334" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -387,13 +414,15 @@
     <col min="3" max="3" width="7.1640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10" customWidth="1"/>
-    <col min="8" max="9" width="23.5" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="23.5" customWidth="1"/>
+    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="24" customWidth="1"/>
+    <col min="19" max="19" width="18.33203125" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,16 +451,43 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -460,12 +516,39 @@
         <v>0.8</v>
       </c>
       <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M2" s="1">
+        <v>6</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P2" s="1">
         <v>0.1</v>
       </c>
-      <c r="K2">
+      <c r="Q2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="T2">
         <v>1E-3</v>
       </c>
-      <c r="L2" s="1">
+      <c r="U2" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>

</xml_diff>